<commit_message>
Checklist-Japanese - sync with engish version 1.1.1.3
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-Japanese_1.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-Japanese_1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\owasp-mstg\owasp-mstg-ja-20181106-2139X\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61DD0A6-97D8-4CED-811F-C284756744E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50CECD5-AED2-4321-B39B-DAFC3AAD2D7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="948" yWindow="144" windowWidth="22020" windowHeight="12108" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="168" yWindow="72" windowWidth="22020" windowHeight="12108" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="303">
   <si>
     <t>ID</t>
   </si>
@@ -1112,13 +1112,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>バックグラウンド時にアプリはビューから機密データを削除していることを検証する。</t>
-    <rPh sb="34" eb="36">
-      <t>ケンショウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>アプリは必要以上に長くメモリ内に機密データを保持せず、使用後は明示的にメモリがクリアされていることを検証する。</t>
     <rPh sb="50" eb="52">
       <t>ケンショウ</t>
@@ -1786,6 +1779,25 @@
   </si>
   <si>
     <t>translate ver. 1.1.1.2 into Japanese</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1.1.1.3</t>
+  </si>
+  <si>
+    <t>Synchronizing the requirements wording in excel with the MASVS
+changes:
+2.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating the link 2.12 for IOS </t>
+  </si>
+  <si>
+    <t>バックグラウンドへ移動した際にアプリはビューから機密データを削除している。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>translate ver. 1.1.1.3 into Japanese</t>
     <phoneticPr fontId="12"/>
   </si>
 </sst>
@@ -2623,7 +2635,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2858,9 +2870,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2892,148 +2901,148 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="9" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -4331,48 +4340,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="123" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="117"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="125"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="118"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="120"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="128"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="118"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="120"/>
+      <c r="B4" s="126"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="128"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="118"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="120"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="128"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="118"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="120"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="128"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="118"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="120"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="128"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="121"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="123"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="131"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="124" t="s">
+      <c r="B9" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="125"/>
-      <c r="D9" s="126"/>
+      <c r="C9" s="119"/>
+      <c r="D9" s="120"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="20" t="s">
@@ -4382,20 +4391,20 @@
       <c r="D10" s="22"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="111" t="s">
+      <c r="B11" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="112"/>
+      <c r="C11" s="118"/>
       <c r="D11" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="111" t="s">
-        <v>293</v>
-      </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="158" t="str">
+      <c r="B12" s="117" t="s">
+        <v>292</v>
+      </c>
+      <c r="C12" s="118"/>
+      <c r="D12" s="111" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
 MASVS_VERSION,
@@ -4404,20 +4413,20 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="111" t="s">
-        <v>294</v>
-      </c>
-      <c r="C13" s="112"/>
+      <c r="B13" s="117" t="s">
+        <v>293</v>
+      </c>
+      <c r="C13" s="118"/>
       <c r="D13" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="111" t="s">
+      <c r="B14" s="117" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="112"/>
-      <c r="D14" s="158" t="str">
+      <c r="C14" s="118"/>
+      <c r="D14" s="111" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
 MSTG_VERSION,
@@ -4426,69 +4435,69 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="127" t="s">
+      <c r="B15" s="133" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="128"/>
-      <c r="D15" s="129"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="135"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="111" t="s">
+      <c r="B16" s="117" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="112"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="23"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="113" t="s">
+      <c r="B17" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="114"/>
+      <c r="C17" s="122"/>
       <c r="D17" s="23"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="111" t="s">
+      <c r="B18" s="117" t="s">
         <v>145</v>
       </c>
-      <c r="C18" s="112"/>
+      <c r="C18" s="118"/>
       <c r="D18" s="23"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="111" t="s">
+      <c r="B19" s="117" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="112"/>
+      <c r="C19" s="118"/>
       <c r="D19" s="23"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="111" t="s">
+      <c r="B20" s="117" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="112"/>
+      <c r="C20" s="118"/>
       <c r="D20" s="23"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="111" t="s">
+      <c r="B21" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="C21" s="112"/>
+      <c r="C21" s="118"/>
       <c r="D21" s="23" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="111" t="s">
+      <c r="B22" s="117" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="112"/>
+      <c r="C22" s="118"/>
       <c r="D22" s="23" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="125"/>
-      <c r="C23" s="125"/>
-      <c r="D23" s="126"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="120"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="20" t="s">
@@ -4505,37 +4514,37 @@
       <c r="D25" s="23"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="111" t="s">
+      <c r="B26" s="117" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="112"/>
+      <c r="C26" s="118"/>
       <c r="D26" s="23"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="111" t="s">
+      <c r="B27" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="C27" s="112"/>
+      <c r="C27" s="118"/>
       <c r="D27" s="23"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="111" t="s">
+      <c r="B28" s="117" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="112"/>
+      <c r="C28" s="118"/>
       <c r="D28" s="23"/>
     </row>
     <row r="29" spans="2:4" ht="52.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="134" t="s">
+      <c r="B29" s="121" t="s">
         <v>156</v>
       </c>
-      <c r="C29" s="112"/>
+      <c r="C29" s="118"/>
       <c r="D29" s="23"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="125"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="126"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="120"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="20" t="s">
@@ -4552,37 +4561,37 @@
       <c r="D32" s="23"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="111" t="s">
+      <c r="B33" s="117" t="s">
         <v>158</v>
       </c>
-      <c r="C33" s="112"/>
+      <c r="C33" s="118"/>
       <c r="D33" s="23"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="111" t="s">
+      <c r="B34" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="C34" s="112"/>
+      <c r="C34" s="118"/>
       <c r="D34" s="23"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" s="111" t="s">
+      <c r="B35" s="117" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="112"/>
+      <c r="C35" s="118"/>
       <c r="D35" s="23"/>
     </row>
     <row r="36" spans="2:4" ht="52.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="134" t="s">
+      <c r="B36" s="121" t="s">
         <v>160</v>
       </c>
-      <c r="C36" s="112"/>
+      <c r="C36" s="118"/>
       <c r="D36" s="23"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" s="125"/>
-      <c r="C37" s="125"/>
-      <c r="D37" s="126"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="120"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="20" t="s">
@@ -4592,97 +4601,100 @@
       <c r="D38" s="22"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" s="130"/>
-      <c r="C39" s="131"/>
-      <c r="D39" s="132"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="116"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="113" t="s">
+      <c r="B40" s="112" t="s">
         <v>162</v>
       </c>
-      <c r="C40" s="133"/>
+      <c r="C40" s="113"/>
       <c r="D40" s="26"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41" s="113" t="s">
+      <c r="B41" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="C41" s="133"/>
+      <c r="C41" s="113"/>
       <c r="D41" s="26"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="113" t="s">
+      <c r="B42" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="C42" s="133"/>
+      <c r="C42" s="113"/>
       <c r="D42" s="26"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="113" t="s">
+      <c r="B43" s="112" t="s">
         <v>165</v>
       </c>
-      <c r="C43" s="133"/>
+      <c r="C43" s="113"/>
       <c r="D43" s="27"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" s="113" t="s">
+      <c r="B44" s="112" t="s">
         <v>166</v>
       </c>
-      <c r="C44" s="133"/>
+      <c r="C44" s="113"/>
       <c r="D44" s="26"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" s="130"/>
-      <c r="C45" s="131"/>
-      <c r="D45" s="132"/>
+      <c r="B45" s="114"/>
+      <c r="C45" s="115"/>
+      <c r="D45" s="116"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="113" t="s">
+      <c r="B46" s="112" t="s">
         <v>162</v>
       </c>
-      <c r="C46" s="133"/>
+      <c r="C46" s="113"/>
       <c r="D46" s="26"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B47" s="113" t="s">
+      <c r="B47" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="C47" s="133"/>
+      <c r="C47" s="113"/>
       <c r="D47" s="26"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" s="113" t="s">
+      <c r="B48" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="C48" s="133"/>
+      <c r="C48" s="113"/>
       <c r="D48" s="26"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="113" t="s">
+      <c r="B49" s="112" t="s">
         <v>165</v>
       </c>
-      <c r="C49" s="133"/>
+      <c r="C49" s="113"/>
       <c r="D49" s="27"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" s="113" t="s">
+      <c r="B50" s="112" t="s">
         <v>166</v>
       </c>
-      <c r="C50" s="133"/>
+      <c r="C50" s="113"/>
       <c r="D50" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B39:D39"/>
@@ -4697,19 +4709,16 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <phoneticPr fontId="12"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4755,11 +4764,11 @@
       <c r="F3" s="31"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.5">
-      <c r="B4" s="151"/>
-      <c r="C4" s="151"/>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
+      <c r="B4" s="136"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
     </row>
     <row r="5" spans="2:24" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="32"/>
@@ -4774,16 +4783,16 @@
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
       <c r="F6" s="33"/>
-      <c r="G6" s="135" t="s">
+      <c r="G6" s="146" t="s">
         <v>168</v>
       </c>
-      <c r="H6" s="136"/>
-      <c r="I6" s="137"/>
-      <c r="V6" s="135" t="s">
+      <c r="H6" s="147"/>
+      <c r="I6" s="148"/>
+      <c r="V6" s="146" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="136"/>
-      <c r="X6" s="137"/>
+      <c r="W6" s="147"/>
+      <c r="X6" s="148"/>
     </row>
     <row r="7" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="34"/>
@@ -4798,18 +4807,18 @@
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="138">
+      <c r="G8" s="137">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="139"/>
-      <c r="I8" s="140"/>
-      <c r="V8" s="138">
+      <c r="H8" s="138"/>
+      <c r="I8" s="139"/>
+      <c r="V8" s="137">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="139"/>
-      <c r="X8" s="140"/>
+      <c r="W8" s="138"/>
+      <c r="X8" s="139"/>
     </row>
     <row r="9" spans="2:24" ht="91.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="33"/>
@@ -4817,12 +4826,12 @@
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
-      <c r="G9" s="141"/>
-      <c r="H9" s="142"/>
-      <c r="I9" s="143"/>
-      <c r="V9" s="141"/>
-      <c r="W9" s="142"/>
-      <c r="X9" s="143"/>
+      <c r="G9" s="140"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="142"/>
+      <c r="V9" s="140"/>
+      <c r="W9" s="141"/>
+      <c r="X9" s="142"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="34"/>
@@ -4830,12 +4839,12 @@
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
-      <c r="G10" s="141"/>
-      <c r="H10" s="142"/>
-      <c r="I10" s="143"/>
-      <c r="V10" s="141"/>
-      <c r="W10" s="142"/>
-      <c r="X10" s="143"/>
+      <c r="G10" s="140"/>
+      <c r="H10" s="141"/>
+      <c r="I10" s="142"/>
+      <c r="V10" s="140"/>
+      <c r="W10" s="141"/>
+      <c r="X10" s="142"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="34"/>
@@ -4843,19 +4852,19 @@
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
-      <c r="G11" s="144"/>
-      <c r="H11" s="145"/>
-      <c r="I11" s="146"/>
-      <c r="V11" s="144"/>
-      <c r="W11" s="145"/>
-      <c r="X11" s="146"/>
+      <c r="G11" s="143"/>
+      <c r="H11" s="144"/>
+      <c r="I11" s="145"/>
+      <c r="V11" s="143"/>
+      <c r="W11" s="144"/>
+      <c r="X11" s="145"/>
     </row>
     <row r="12" spans="2:24" ht="16.05" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="147"/>
-      <c r="C12" s="147"/>
-      <c r="D12" s="147"/>
-      <c r="E12" s="147"/>
-      <c r="F12" s="147"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="149"/>
+      <c r="D12" s="149"/>
+      <c r="E12" s="149"/>
+      <c r="F12" s="149"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B13" s="35"/>
@@ -4879,11 +4888,11 @@
       <c r="F15" s="34"/>
     </row>
     <row r="16" spans="2:24" ht="16.05" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="147"/>
-      <c r="C16" s="147"/>
-      <c r="D16" s="147"/>
-      <c r="E16" s="147"/>
-      <c r="F16" s="147"/>
+      <c r="B16" s="149"/>
+      <c r="C16" s="149"/>
+      <c r="D16" s="149"/>
+      <c r="E16" s="149"/>
+      <c r="F16" s="149"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B17" s="35"/>
@@ -4931,18 +4940,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="41" spans="3:11" x14ac:dyDescent="0.5">
-      <c r="D41" s="148" t="s">
+      <c r="D41" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="149"/>
-      <c r="F41" s="149"/>
-      <c r="G41" s="150"/>
-      <c r="H41" s="148" t="s">
+      <c r="E41" s="151"/>
+      <c r="F41" s="151"/>
+      <c r="G41" s="152"/>
+      <c r="H41" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="I41" s="149"/>
-      <c r="J41" s="149"/>
-      <c r="K41" s="150"/>
+      <c r="I41" s="151"/>
+      <c r="J41" s="151"/>
+      <c r="K41" s="152"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.5">
       <c r="D42" s="39" t="s">
@@ -5268,15 +5277,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:K41"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:K41"/>
   </mergeCells>
   <phoneticPr fontId="12"/>
   <conditionalFormatting sqref="F14">
@@ -5338,16 +5347,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="21.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="153" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="49" t="s">
@@ -5365,10 +5374,10 @@
       <c r="F3" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="154" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="153"/>
+      <c r="H3" s="154"/>
       <c r="I3" s="52" t="s">
         <v>186</v>
       </c>
@@ -5388,7 +5397,7 @@
       <c r="I4" s="56"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="107" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="57" t="s">
@@ -5408,7 +5417,7 @@
       <c r="I5" s="62"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="107" t="s">
         <v>112</v>
       </c>
       <c r="C6" s="57" t="s">
@@ -5428,7 +5437,7 @@
       <c r="I6" s="62"/>
     </row>
     <row r="7" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="107" t="s">
         <v>111</v>
       </c>
       <c r="C7" s="57" t="s">
@@ -5448,7 +5457,7 @@
       <c r="I7" s="62"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="107" t="s">
         <v>110</v>
       </c>
       <c r="C8" s="57" t="s">
@@ -5468,7 +5477,7 @@
       <c r="I8" s="62"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C9" s="57" t="s">
@@ -5488,7 +5497,7 @@
       <c r="I9" s="62"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="107" t="s">
         <v>108</v>
       </c>
       <c r="C10" s="57" t="s">
@@ -5508,7 +5517,7 @@
       <c r="I10" s="62"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="107" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="57" t="s">
@@ -5528,7 +5537,7 @@
       <c r="I11" s="62"/>
     </row>
     <row r="12" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="107" t="s">
         <v>107</v>
       </c>
       <c r="C12" s="57" t="s">
@@ -5548,7 +5557,7 @@
       <c r="I12" s="62"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="107" t="s">
         <v>106</v>
       </c>
       <c r="C13" s="57" t="s">
@@ -5568,7 +5577,7 @@
       <c r="I13" s="62"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="108" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="57" t="s">
@@ -5602,7 +5611,7 @@
       <c r="I15" s="69"/>
     </row>
     <row r="16" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="107" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="57" t="s">
@@ -5626,7 +5635,7 @@
       <c r="I16" s="62"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="107" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="57" t="s">
@@ -5646,7 +5655,7 @@
       <c r="I17" s="72"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="107" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="57" t="s">
@@ -5670,7 +5679,7 @@
       <c r="I18" s="62"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="107" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="57" t="s">
@@ -5694,7 +5703,7 @@
       <c r="I19" s="62"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="107" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="57" t="s">
@@ -5718,7 +5727,7 @@
       <c r="I20" s="62"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="108" t="s">
+      <c r="B21" s="107" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="57" t="s">
@@ -5742,7 +5751,7 @@
       <c r="I21" s="62"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="108" t="s">
+      <c r="B22" s="107" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="57" t="s">
@@ -5766,7 +5775,7 @@
       <c r="I22" s="62"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="107" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="57" t="s">
@@ -5790,11 +5799,11 @@
       <c r="I23" s="62"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="108" t="s">
+      <c r="B24" s="107" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="57" t="s">
-        <v>207</v>
+        <v>301</v>
       </c>
       <c r="D24" s="73"/>
       <c r="E24" s="59" t="s">
@@ -5814,11 +5823,11 @@
       <c r="I24" s="62"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" s="108" t="s">
+      <c r="B25" s="107" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D25" s="73"/>
       <c r="E25" s="59" t="s">
@@ -5838,11 +5847,11 @@
       <c r="I25" s="62"/>
     </row>
     <row r="26" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="108" t="s">
+      <c r="B26" s="107" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="57" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D26" s="73"/>
       <c r="E26" s="59" t="s">
@@ -5862,11 +5871,11 @@
       <c r="I26" s="62"/>
     </row>
     <row r="27" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="108" t="s">
+      <c r="B27" s="107" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="57" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D27" s="73"/>
       <c r="E27" s="59" t="s">
@@ -5890,7 +5899,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="68"/>
@@ -5900,11 +5909,11 @@
       <c r="I28" s="69"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="108" t="s">
+      <c r="B29" s="107" t="s">
         <v>15</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D29" s="58" t="s">
         <v>3</v>
@@ -5924,11 +5933,11 @@
       <c r="I29" s="62"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="108" t="s">
+      <c r="B30" s="107" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D30" s="58" t="s">
         <v>3</v>
@@ -5948,11 +5957,11 @@
       <c r="I30" s="62"/>
     </row>
     <row r="31" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="108" t="s">
+      <c r="B31" s="107" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D31" s="58" t="s">
         <v>3</v>
@@ -5972,11 +5981,11 @@
       <c r="I31" s="62"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="108" t="s">
+      <c r="B32" s="107" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D32" s="58" t="s">
         <v>3</v>
@@ -5996,11 +6005,11 @@
       <c r="I32" s="62"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="108" t="s">
+      <c r="B33" s="107" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D33" s="58" t="s">
         <v>3</v>
@@ -6020,11 +6029,11 @@
       <c r="I33" s="62"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="108" t="s">
+      <c r="B34" s="107" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D34" s="58" t="s">
         <v>3</v>
@@ -6048,7 +6057,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D35" s="67"/>
       <c r="E35" s="68"/>
@@ -6058,11 +6067,11 @@
       <c r="I35" s="69"/>
     </row>
     <row r="36" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="108" t="s">
+      <c r="B36" s="107" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="74" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D36" s="58" t="s">
         <v>3</v>
@@ -6082,11 +6091,11 @@
       <c r="I36" s="62"/>
     </row>
     <row r="37" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" s="108" t="s">
+      <c r="B37" s="107" t="s">
         <v>44</v>
       </c>
       <c r="C37" s="74" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D37" s="58" t="s">
         <v>3</v>
@@ -6106,11 +6115,11 @@
       <c r="I37" s="62"/>
     </row>
     <row r="38" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" s="108" t="s">
+      <c r="B38" s="107" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="74" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D38" s="58" t="s">
         <v>3</v>
@@ -6131,11 +6140,11 @@
       <c r="K38" s="75"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" s="108" t="s">
+      <c r="B39" s="107" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D39" s="58"/>
       <c r="E39" s="59"/>
@@ -6152,11 +6161,11 @@
       <c r="K39" s="75"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="108" t="s">
+      <c r="B40" s="107" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="74" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D40" s="58" t="s">
         <v>3</v>
@@ -6176,11 +6185,11 @@
       <c r="I40" s="62"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41" s="108" t="s">
+      <c r="B41" s="107" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="74" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>3</v>
@@ -6200,11 +6209,11 @@
       <c r="I41" s="62"/>
     </row>
     <row r="42" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="108" t="s">
+      <c r="B42" s="107" t="s">
         <v>47</v>
       </c>
       <c r="C42" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D42" s="58" t="s">
         <v>3</v>
@@ -6224,11 +6233,11 @@
       <c r="I42" s="76"/>
     </row>
     <row r="43" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="108" t="s">
+      <c r="B43" s="107" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D43" s="73"/>
       <c r="E43" s="59" t="s">
@@ -6248,11 +6257,11 @@
       <c r="I43" s="62"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" s="108" t="s">
+      <c r="B44" s="107" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D44" s="73"/>
       <c r="E44" s="59" t="s">
@@ -6272,11 +6281,11 @@
       <c r="I44" s="62"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" s="108" t="s">
+      <c r="B45" s="107" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="74" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D45" s="73"/>
       <c r="E45" s="59" t="s">
@@ -6296,11 +6305,11 @@
       <c r="I45" s="62"/>
     </row>
     <row r="46" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="108" t="s">
+      <c r="B46" s="107" t="s">
         <v>91</v>
       </c>
       <c r="C46" s="74" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D46" s="73"/>
       <c r="E46" s="59" t="s">
@@ -6325,7 +6334,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D47" s="67"/>
       <c r="E47" s="68"/>
@@ -6335,11 +6344,11 @@
       <c r="I47" s="69"/>
     </row>
     <row r="48" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" s="108" t="s">
+      <c r="B48" s="107" t="s">
         <v>29</v>
       </c>
       <c r="C48" s="74" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D48" s="58" t="s">
         <v>3</v>
@@ -6359,11 +6368,11 @@
       <c r="I48" s="62"/>
     </row>
     <row r="49" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="108" t="s">
+      <c r="B49" s="107" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="74" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D49" s="58" t="s">
         <v>3</v>
@@ -6383,11 +6392,11 @@
       <c r="I49" s="62"/>
     </row>
     <row r="50" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" s="108" t="s">
+      <c r="B50" s="107" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D50" s="58" t="s">
         <v>3</v>
@@ -6407,11 +6416,11 @@
       <c r="I50" s="78"/>
     </row>
     <row r="51" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="108" t="s">
+      <c r="B51" s="107" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="74" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D51" s="73"/>
       <c r="E51" s="59" t="s">
@@ -6431,11 +6440,11 @@
       <c r="I51" s="62"/>
     </row>
     <row r="52" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" s="108" t="s">
+      <c r="B52" s="107" t="s">
         <v>31</v>
       </c>
       <c r="C52" s="74" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D52" s="73"/>
       <c r="E52" s="59" t="s">
@@ -6455,11 +6464,11 @@
       <c r="I52" s="62"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="108" t="s">
+      <c r="B53" s="107" t="s">
         <v>105</v>
       </c>
       <c r="C53" s="74" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D53" s="73"/>
       <c r="E53" s="59" t="s">
@@ -6483,7 +6492,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D54" s="67"/>
       <c r="E54" s="68"/>
@@ -6493,11 +6502,11 @@
       <c r="I54" s="69"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55" s="108" t="s">
+      <c r="B55" s="107" t="s">
         <v>50</v>
       </c>
       <c r="C55" s="74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D55" s="58" t="s">
         <v>3</v>
@@ -6517,11 +6526,11 @@
       <c r="I55" s="62"/>
     </row>
     <row r="56" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B56" s="108" t="s">
+      <c r="B56" s="107" t="s">
         <v>51</v>
       </c>
       <c r="C56" s="74" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D56" s="58" t="s">
         <v>3</v>
@@ -6541,11 +6550,11 @@
       <c r="I56" s="62"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57" s="108" t="s">
+      <c r="B57" s="107" t="s">
         <v>52</v>
       </c>
       <c r="C57" s="74" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D57" s="58" t="s">
         <v>3</v>
@@ -6565,11 +6574,11 @@
       <c r="I57" s="62"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B58" s="108" t="s">
+      <c r="B58" s="107" t="s">
         <v>53</v>
       </c>
       <c r="C58" s="74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D58" s="58" t="s">
         <v>3</v>
@@ -6589,11 +6598,11 @@
       <c r="I58" s="62"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59" s="108" t="s">
+      <c r="B59" s="107" t="s">
         <v>54</v>
       </c>
       <c r="C59" s="74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D59" s="58" t="s">
         <v>3</v>
@@ -6613,11 +6622,11 @@
       <c r="I59" s="62"/>
     </row>
     <row r="60" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B60" s="108" t="s">
+      <c r="B60" s="107" t="s">
         <v>55</v>
       </c>
       <c r="C60" s="74" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D60" s="58" t="s">
         <v>3</v>
@@ -6637,11 +6646,11 @@
       <c r="I60" s="62"/>
     </row>
     <row r="61" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B61" s="108" t="s">
+      <c r="B61" s="107" t="s">
         <v>104</v>
       </c>
       <c r="C61" s="74" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D61" s="58" t="s">
         <v>3</v>
@@ -6661,11 +6670,11 @@
       <c r="I61" s="62"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B62" s="108" t="s">
+      <c r="B62" s="107" t="s">
         <v>103</v>
       </c>
       <c r="C62" s="74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D62" s="58" t="s">
         <v>3</v>
@@ -6689,7 +6698,7 @@
         <v>33</v>
       </c>
       <c r="C63" s="66" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D63" s="67"/>
       <c r="E63" s="68"/>
@@ -6699,11 +6708,11 @@
       <c r="I63" s="69"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B64" s="108" t="s">
+      <c r="B64" s="107" t="s">
         <v>56</v>
       </c>
       <c r="C64" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D64" s="58" t="s">
         <v>3</v>
@@ -6723,11 +6732,11 @@
       <c r="I64" s="62"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B65" s="108" t="s">
+      <c r="B65" s="107" t="s">
         <v>34</v>
       </c>
       <c r="C65" s="57" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D65" s="58" t="s">
         <v>3</v>
@@ -6747,11 +6756,11 @@
       <c r="I65" s="62"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B66" s="108" t="s">
+      <c r="B66" s="107" t="s">
         <v>57</v>
       </c>
       <c r="C66" s="57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D66" s="58" t="s">
         <v>3</v>
@@ -6771,11 +6780,11 @@
       <c r="I66" s="62"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B67" s="108" t="s">
+      <c r="B67" s="107" t="s">
         <v>58</v>
       </c>
       <c r="C67" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D67" s="58" t="s">
         <v>3</v>
@@ -6795,11 +6804,11 @@
       <c r="I67" s="62"/>
     </row>
     <row r="68" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B68" s="108" t="s">
+      <c r="B68" s="107" t="s">
         <v>59</v>
       </c>
       <c r="C68" s="57" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D68" s="58" t="s">
         <v>3</v>
@@ -6819,11 +6828,11 @@
       <c r="I68" s="62"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B69" s="108" t="s">
+      <c r="B69" s="107" t="s">
         <v>35</v>
       </c>
       <c r="C69" s="57" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D69" s="58" t="s">
         <v>3</v>
@@ -6843,11 +6852,11 @@
       <c r="I69" s="62"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B70" s="108" t="s">
+      <c r="B70" s="107" t="s">
         <v>36</v>
       </c>
       <c r="C70" s="57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D70" s="58" t="s">
         <v>3</v>
@@ -6867,11 +6876,11 @@
       <c r="I70" s="62"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B71" s="108" t="s">
+      <c r="B71" s="107" t="s">
         <v>37</v>
       </c>
       <c r="C71" s="57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D71" s="58" t="s">
         <v>3</v>
@@ -6892,11 +6901,11 @@
       <c r="J71" s="80"/>
     </row>
     <row r="72" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B72" s="108" t="s">
+      <c r="B72" s="107" t="s">
         <v>93</v>
       </c>
       <c r="C72" s="57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D72" s="58" t="s">
         <v>3</v>
@@ -6957,7 +6966,7 @@
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" s="86" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C77" s="61"/>
       <c r="D77" s="38"/>
@@ -6969,10 +6978,10 @@
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="C78" s="88" t="s">
         <v>277</v>
-      </c>
-      <c r="C78" s="88" t="s">
-        <v>278</v>
       </c>
       <c r="D78" s="38"/>
       <c r="E78" s="38"/>
@@ -6986,7 +6995,7 @@
         <v>68</v>
       </c>
       <c r="C79" s="90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D79" s="38"/>
       <c r="E79" s="38"/>
@@ -7000,7 +7009,7 @@
         <v>69</v>
       </c>
       <c r="C80" s="90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D80" s="38"/>
       <c r="E80" s="38"/>
@@ -7014,7 +7023,7 @@
         <v>64</v>
       </c>
       <c r="C81" s="90" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D81" s="38"/>
       <c r="E81" s="38"/>
@@ -7108,7 +7117,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="21.6" x14ac:dyDescent="0.6">
       <c r="B1" s="91" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C1" s="61"/>
       <c r="D1" s="38"/>
@@ -7129,7 +7138,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D3" s="51" t="s">
         <v>38</v>
@@ -7138,7 +7147,7 @@
         <v>184</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G3" s="52" t="s">
         <v>186</v>
@@ -7147,7 +7156,7 @@
     <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="65"/>
       <c r="C4" s="66" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D4" s="67"/>
       <c r="E4" s="67"/>
@@ -7155,11 +7164,11 @@
       <c r="G4" s="69"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="107" t="s">
         <v>113</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D5" s="92" t="s">
         <v>3</v>
@@ -7177,11 +7186,11 @@
       <c r="G5" s="62"/>
     </row>
     <row r="6" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="107" t="s">
         <v>114</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D6" s="92" t="s">
         <v>3</v>
@@ -7200,11 +7209,11 @@
       <c r="G6" s="62"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="107" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="92" t="s">
         <v>3</v>
@@ -7222,11 +7231,11 @@
       <c r="G7" s="62"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="107" t="s">
         <v>116</v>
       </c>
       <c r="C8" s="74" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D8" s="92" t="s">
         <v>3</v>
@@ -7244,11 +7253,11 @@
       <c r="G8" s="62"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="107" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D9" s="92" t="s">
         <v>3</v>
@@ -7266,11 +7275,11 @@
       <c r="G9" s="62"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="107" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="74" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D10" s="92" t="s">
         <v>3</v>
@@ -7288,11 +7297,11 @@
       <c r="G10" s="62"/>
     </row>
     <row r="11" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="107" t="s">
         <v>119</v>
       </c>
       <c r="C11" s="74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D11" s="92" t="s">
         <v>3</v>
@@ -7306,11 +7315,11 @@
       <c r="G11" s="62"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="107" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="74" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D12" s="92" t="s">
         <v>3</v>
@@ -7324,11 +7333,11 @@
       <c r="G12" s="62"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="107" t="s">
         <v>95</v>
       </c>
       <c r="C13" s="74" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D13" s="92" t="s">
         <v>3</v>
@@ -7348,7 +7357,7 @@
     <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="65"/>
       <c r="C14" s="66" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D14" s="67"/>
       <c r="E14" s="67"/>
@@ -7356,11 +7365,11 @@
       <c r="G14" s="69"/>
     </row>
     <row r="15" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="108" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="74" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D15" s="92" t="s">
         <v>3</v>
@@ -7380,7 +7389,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="65"/>
       <c r="C16" s="66" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D16" s="67"/>
       <c r="E16" s="67"/>
@@ -7388,11 +7397,11 @@
       <c r="G16" s="69"/>
     </row>
     <row r="17" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="107" t="s">
         <v>121</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>3</v>
@@ -7410,11 +7419,11 @@
       <c r="G17" s="62"/>
     </row>
     <row r="18" spans="2:7" ht="52.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="107" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="74" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D18" s="92" t="s">
         <v>3</v>
@@ -7453,7 +7462,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="86" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C22" s="61"/>
       <c r="D22" s="38"/>
@@ -7463,10 +7472,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" s="88" t="s">
         <v>277</v>
-      </c>
-      <c r="C23" s="88" t="s">
-        <v>278</v>
       </c>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
@@ -7478,7 +7487,7 @@
         <v>68</v>
       </c>
       <c r="C24" s="90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D24" s="38"/>
       <c r="E24" s="38"/>
@@ -7490,7 +7499,7 @@
         <v>69</v>
       </c>
       <c r="C25" s="90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="38"/>
@@ -7502,7 +7511,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="90" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D26" s="38"/>
       <c r="E26" s="38"/>
@@ -7571,7 +7580,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="21.6" x14ac:dyDescent="0.6">
       <c r="B1" s="93" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -7590,10 +7599,10 @@
       <c r="F3" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="154" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="154"/>
+      <c r="H3" s="155"/>
       <c r="I3" s="52" t="s">
         <v>186</v>
       </c>
@@ -7613,7 +7622,7 @@
       <c r="I4" s="56"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="107" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="57" t="s">
@@ -7633,7 +7642,7 @@
       <c r="I5" s="62"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="107" t="s">
         <v>112</v>
       </c>
       <c r="C6" s="57" t="s">
@@ -7653,7 +7662,7 @@
       <c r="I6" s="62"/>
     </row>
     <row r="7" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="107" t="s">
         <v>111</v>
       </c>
       <c r="C7" s="57" t="s">
@@ -7673,7 +7682,7 @@
       <c r="I7" s="62"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="107" t="s">
         <v>110</v>
       </c>
       <c r="C8" s="57" t="s">
@@ -7693,7 +7702,7 @@
       <c r="I8" s="62"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C9" s="57" t="s">
@@ -7713,7 +7722,7 @@
       <c r="I9" s="62"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="107" t="s">
         <v>108</v>
       </c>
       <c r="C10" s="57" t="s">
@@ -7733,7 +7742,7 @@
       <c r="I10" s="62"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="107" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="57" t="s">
@@ -7753,7 +7762,7 @@
       <c r="I11" s="62"/>
     </row>
     <row r="12" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="107" t="s">
         <v>107</v>
       </c>
       <c r="C12" s="57" t="s">
@@ -7773,7 +7782,7 @@
       <c r="I12" s="62"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="107" t="s">
         <v>106</v>
       </c>
       <c r="C13" s="57" t="s">
@@ -7793,7 +7802,7 @@
       <c r="I13" s="62"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="108" t="s">
+      <c r="B14" s="107" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="57" t="s">
@@ -7827,7 +7836,7 @@
       <c r="I15" s="69"/>
     </row>
     <row r="16" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="107" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="57" t="s">
@@ -7851,7 +7860,7 @@
       <c r="I16" s="62"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="107" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="57" t="s">
@@ -7871,7 +7880,7 @@
       <c r="I17" s="62"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="107" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="57" t="s">
@@ -7895,7 +7904,7 @@
       <c r="I18" s="62"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="107" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="57" t="s">
@@ -7919,7 +7928,7 @@
       <c r="I19" s="62"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="107" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="57" t="s">
@@ -7943,7 +7952,7 @@
       <c r="I20" s="62"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="108" t="s">
+      <c r="B21" s="107" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="57" t="s">
@@ -7967,7 +7976,7 @@
       <c r="I21" s="62"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="108" t="s">
+      <c r="B22" s="107" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="57" t="s">
@@ -7991,7 +8000,7 @@
       <c r="I22" s="62"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="107" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="57" t="s">
@@ -8015,11 +8024,11 @@
       <c r="I23" s="62"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="108" t="s">
+      <c r="B24" s="107" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="57" t="s">
-        <v>207</v>
+        <v>301</v>
       </c>
       <c r="D24" s="73"/>
       <c r="E24" s="59" t="s">
@@ -8039,11 +8048,11 @@
       <c r="I24" s="62"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" s="108" t="s">
+      <c r="B25" s="107" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D25" s="73"/>
       <c r="E25" s="59" t="s">
@@ -8063,11 +8072,11 @@
       <c r="I25" s="62"/>
     </row>
     <row r="26" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="108" t="s">
+      <c r="B26" s="107" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="57" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D26" s="73"/>
       <c r="E26" s="59" t="s">
@@ -8088,11 +8097,11 @@
       <c r="J26" s="96"/>
     </row>
     <row r="27" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="108" t="s">
+      <c r="B27" s="107" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="57" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D27" s="73"/>
       <c r="E27" s="59" t="s">
@@ -8101,12 +8110,12 @@
       <c r="F27" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="97" t="str">
-        <f>HYPERLINK(CONCATENATE(
-BASE_URL,
-"0x06f-Testing-Local-Authentication.md#local-authentication-on-ios"),
-"Testing Local Authentication")</f>
-        <v>Testing Local Authentication</v>
+      <c r="G27" s="70" t="str">
+        <f>HYPERLINK(CONCATENATE(
+BASE_URL,
+"0x04i-Testing-user-interaction.md#testing-user-education"),
+"Testing user education")</f>
+        <v>Testing user education</v>
       </c>
       <c r="H27" s="74"/>
       <c r="I27" s="62"/>
@@ -8117,7 +8126,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="68"/>
@@ -8127,11 +8136,11 @@
       <c r="I28" s="69"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="108" t="s">
+      <c r="B29" s="107" t="s">
         <v>15</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D29" s="58" t="s">
         <v>3</v>
@@ -8151,11 +8160,11 @@
       <c r="I29" s="62"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="108" t="s">
+      <c r="B30" s="107" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D30" s="58" t="s">
         <v>3</v>
@@ -8175,11 +8184,11 @@
       <c r="I30" s="62"/>
     </row>
     <row r="31" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="108" t="s">
+      <c r="B31" s="107" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D31" s="58" t="s">
         <v>3</v>
@@ -8199,11 +8208,11 @@
       <c r="I31" s="62"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="108" t="s">
+      <c r="B32" s="107" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D32" s="58" t="s">
         <v>3</v>
@@ -8223,11 +8232,11 @@
       <c r="I32" s="62"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="108" t="s">
+      <c r="B33" s="107" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D33" s="58" t="s">
         <v>3</v>
@@ -8247,11 +8256,11 @@
       <c r="I33" s="62"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="108" t="s">
+      <c r="B34" s="107" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D34" s="58" t="s">
         <v>3</v>
@@ -8275,7 +8284,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D35" s="67"/>
       <c r="E35" s="68"/>
@@ -8285,11 +8294,11 @@
       <c r="I35" s="69"/>
     </row>
     <row r="36" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="108" t="s">
+      <c r="B36" s="107" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="74" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D36" s="58" t="s">
         <v>3</v>
@@ -8309,11 +8318,11 @@
       <c r="I36" s="62"/>
     </row>
     <row r="37" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" s="108" t="s">
+      <c r="B37" s="107" t="s">
         <v>44</v>
       </c>
       <c r="C37" s="74" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D37" s="58" t="s">
         <v>3</v>
@@ -8333,11 +8342,11 @@
       <c r="I37" s="62"/>
     </row>
     <row r="38" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" s="108" t="s">
+      <c r="B38" s="107" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="74" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D38" s="58" t="s">
         <v>3</v>
@@ -8357,11 +8366,11 @@
       <c r="I38" s="62"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" s="108" t="s">
+      <c r="B39" s="107" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D39" s="58"/>
       <c r="E39" s="59"/>
@@ -8379,11 +8388,11 @@
       <c r="K39" s="75"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="108" t="s">
+      <c r="B40" s="107" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="74" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D40" s="58" t="s">
         <v>3</v>
@@ -8404,11 +8413,11 @@
       <c r="K40" s="75"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41" s="108" t="s">
+      <c r="B41" s="107" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="74" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>3</v>
@@ -8428,11 +8437,11 @@
       <c r="I41" s="62"/>
     </row>
     <row r="42" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="108" t="s">
+      <c r="B42" s="107" t="s">
         <v>47</v>
       </c>
       <c r="C42" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D42" s="58" t="s">
         <v>3</v>
@@ -8448,15 +8457,15 @@
 "Testing the Session Timeout")</f>
         <v>Testing the Session Timeout</v>
       </c>
-      <c r="H42" s="98"/>
+      <c r="H42" s="97"/>
       <c r="I42" s="76"/>
     </row>
     <row r="43" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="108" t="s">
+      <c r="B43" s="107" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D43" s="73"/>
       <c r="E43" s="59" t="s">
@@ -8476,11 +8485,11 @@
       <c r="I43" s="62"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" s="108" t="s">
+      <c r="B44" s="107" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D44" s="73"/>
       <c r="E44" s="59" t="s">
@@ -8500,11 +8509,11 @@
       <c r="I44" s="62"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" s="108" t="s">
+      <c r="B45" s="107" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="74" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D45" s="73"/>
       <c r="E45" s="59" t="s">
@@ -8524,11 +8533,11 @@
       <c r="I45" s="62"/>
     </row>
     <row r="46" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="108" t="s">
+      <c r="B46" s="107" t="s">
         <v>91</v>
       </c>
       <c r="C46" s="74" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D46" s="73"/>
       <c r="E46" s="59" t="s">
@@ -8552,7 +8561,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D47" s="67"/>
       <c r="E47" s="68"/>
@@ -8562,11 +8571,11 @@
       <c r="I47" s="69"/>
     </row>
     <row r="48" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" s="108" t="s">
+      <c r="B48" s="107" t="s">
         <v>29</v>
       </c>
       <c r="C48" s="74" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D48" s="58" t="s">
         <v>3</v>
@@ -8592,11 +8601,11 @@
       <c r="I48" s="78"/>
     </row>
     <row r="49" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="108" t="s">
+      <c r="B49" s="107" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="74" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D49" s="58" t="s">
         <v>3</v>
@@ -8622,11 +8631,11 @@
       <c r="I49" s="78"/>
     </row>
     <row r="50" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" s="108" t="s">
+      <c r="B50" s="107" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D50" s="58" t="s">
         <v>3</v>
@@ -8646,11 +8655,11 @@
       <c r="I50" s="78"/>
     </row>
     <row r="51" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="108" t="s">
+      <c r="B51" s="107" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="74" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D51" s="73"/>
       <c r="E51" s="59" t="s">
@@ -8670,11 +8679,11 @@
       <c r="I51" s="62"/>
     </row>
     <row r="52" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" s="108" t="s">
+      <c r="B52" s="107" t="s">
         <v>31</v>
       </c>
       <c r="C52" s="74" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D52" s="73"/>
       <c r="E52" s="59" t="s">
@@ -8694,11 +8703,11 @@
       <c r="I52" s="62"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="108" t="s">
+      <c r="B53" s="107" t="s">
         <v>105</v>
       </c>
       <c r="C53" s="74" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D53" s="73"/>
       <c r="E53" s="59" t="s">
@@ -8722,7 +8731,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D54" s="67"/>
       <c r="E54" s="68"/>
@@ -8732,11 +8741,11 @@
       <c r="I54" s="69"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55" s="108" t="s">
+      <c r="B55" s="107" t="s">
         <v>50</v>
       </c>
       <c r="C55" s="74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D55" s="58" t="s">
         <v>3</v>
@@ -8756,11 +8765,11 @@
       <c r="I55" s="62"/>
     </row>
     <row r="56" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B56" s="108" t="s">
+      <c r="B56" s="107" t="s">
         <v>51</v>
       </c>
       <c r="C56" s="74" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D56" s="58" t="s">
         <v>3</v>
@@ -8780,11 +8789,11 @@
       <c r="I56" s="62"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57" s="108" t="s">
+      <c r="B57" s="107" t="s">
         <v>52</v>
       </c>
       <c r="C57" s="74" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D57" s="58" t="s">
         <v>3</v>
@@ -8804,11 +8813,11 @@
       <c r="I57" s="62"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B58" s="108" t="s">
+      <c r="B58" s="107" t="s">
         <v>53</v>
       </c>
       <c r="C58" s="74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D58" s="58" t="s">
         <v>3</v>
@@ -8828,11 +8837,11 @@
       <c r="I58" s="62"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59" s="108" t="s">
+      <c r="B59" s="107" t="s">
         <v>54</v>
       </c>
       <c r="C59" s="74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D59" s="58" t="s">
         <v>3</v>
@@ -8852,11 +8861,11 @@
       <c r="I59" s="62"/>
     </row>
     <row r="60" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B60" s="108" t="s">
+      <c r="B60" s="107" t="s">
         <v>55</v>
       </c>
       <c r="C60" s="74" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D60" s="58" t="s">
         <v>3</v>
@@ -8876,11 +8885,11 @@
       <c r="I60" s="62"/>
     </row>
     <row r="61" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B61" s="108" t="s">
+      <c r="B61" s="107" t="s">
         <v>104</v>
       </c>
       <c r="C61" s="74" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D61" s="58" t="s">
         <v>3</v>
@@ -8900,11 +8909,11 @@
       <c r="I61" s="62"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B62" s="108" t="s">
+      <c r="B62" s="107" t="s">
         <v>103</v>
       </c>
       <c r="C62" s="74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D62" s="58" t="s">
         <v>3</v>
@@ -8928,7 +8937,7 @@
         <v>33</v>
       </c>
       <c r="C63" s="66" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D63" s="67"/>
       <c r="E63" s="68"/>
@@ -8938,11 +8947,11 @@
       <c r="I63" s="69"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B64" s="108" t="s">
+      <c r="B64" s="107" t="s">
         <v>56</v>
       </c>
       <c r="C64" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D64" s="58" t="s">
         <v>3</v>
@@ -8962,11 +8971,11 @@
       <c r="I64" s="62"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B65" s="108" t="s">
+      <c r="B65" s="107" t="s">
         <v>34</v>
       </c>
       <c r="C65" s="57" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D65" s="58" t="s">
         <v>3</v>
@@ -8986,11 +8995,11 @@
       <c r="I65" s="62"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B66" s="108" t="s">
+      <c r="B66" s="107" t="s">
         <v>57</v>
       </c>
       <c r="C66" s="57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D66" s="58" t="s">
         <v>3</v>
@@ -9010,11 +9019,11 @@
       <c r="I66" s="62"/>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B67" s="108" t="s">
+      <c r="B67" s="107" t="s">
         <v>58</v>
       </c>
       <c r="C67" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D67" s="58" t="s">
         <v>3</v>
@@ -9034,11 +9043,11 @@
       <c r="I67" s="62"/>
     </row>
     <row r="68" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B68" s="108" t="s">
+      <c r="B68" s="107" t="s">
         <v>59</v>
       </c>
       <c r="C68" s="57" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D68" s="58" t="s">
         <v>3</v>
@@ -9058,11 +9067,11 @@
       <c r="I68" s="62"/>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B69" s="108" t="s">
+      <c r="B69" s="107" t="s">
         <v>35</v>
       </c>
       <c r="C69" s="57" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D69" s="58" t="s">
         <v>3</v>
@@ -9082,11 +9091,11 @@
       <c r="I69" s="62"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B70" s="108" t="s">
+      <c r="B70" s="107" t="s">
         <v>36</v>
       </c>
       <c r="C70" s="57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D70" s="58" t="s">
         <v>3</v>
@@ -9106,11 +9115,11 @@
       <c r="I70" s="62"/>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B71" s="108" t="s">
+      <c r="B71" s="107" t="s">
         <v>37</v>
       </c>
       <c r="C71" s="57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D71" s="58" t="s">
         <v>3</v>
@@ -9130,11 +9139,11 @@
       <c r="I71" s="62"/>
     </row>
     <row r="72" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B72" s="108" t="s">
+      <c r="B72" s="107" t="s">
         <v>93</v>
       </c>
       <c r="C72" s="57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D72" s="58" t="s">
         <v>3</v>
@@ -9160,146 +9169,146 @@
       <c r="E73" s="83"/>
       <c r="F73" s="83"/>
       <c r="G73" s="82"/>
-      <c r="H73" s="99"/>
-      <c r="I73" s="100"/>
+      <c r="H73" s="98"/>
+      <c r="I73" s="99"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B74" s="101"/>
-      <c r="C74" s="102"/>
+      <c r="B74" s="100"/>
+      <c r="C74" s="101"/>
       <c r="D74" s="28"/>
       <c r="E74" s="28"/>
       <c r="F74" s="28"/>
-      <c r="G74" s="102"/>
+      <c r="G74" s="101"/>
       <c r="H74" s="61"/>
-      <c r="I74" s="102"/>
+      <c r="I74" s="101"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B75" s="101"/>
-      <c r="C75" s="102"/>
+      <c r="B75" s="100"/>
+      <c r="C75" s="101"/>
       <c r="D75" s="28"/>
       <c r="E75" s="28"/>
       <c r="F75" s="28"/>
-      <c r="G75" s="98"/>
+      <c r="G75" s="97"/>
       <c r="H75" s="61"/>
-      <c r="I75" s="102"/>
+      <c r="I75" s="101"/>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B76" s="101"/>
-      <c r="C76" s="102"/>
+      <c r="B76" s="100"/>
+      <c r="C76" s="101"/>
       <c r="D76" s="28"/>
       <c r="E76" s="28"/>
       <c r="F76" s="28"/>
-      <c r="G76" s="102"/>
+      <c r="G76" s="101"/>
       <c r="H76" s="61"/>
-      <c r="I76" s="102"/>
+      <c r="I76" s="101"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B77" s="103" t="s">
-        <v>276</v>
-      </c>
-      <c r="C77" s="102"/>
+      <c r="B77" s="102" t="s">
+        <v>275</v>
+      </c>
+      <c r="C77" s="101"/>
       <c r="D77" s="28"/>
       <c r="E77" s="28"/>
       <c r="F77" s="28"/>
-      <c r="G77" s="102"/>
+      <c r="G77" s="101"/>
       <c r="H77" s="61"/>
-      <c r="I77" s="102"/>
+      <c r="I77" s="101"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="C78" s="88" t="s">
         <v>277</v>
-      </c>
-      <c r="C78" s="88" t="s">
-        <v>278</v>
       </c>
       <c r="D78" s="28"/>
       <c r="E78" s="28"/>
       <c r="F78" s="28"/>
-      <c r="G78" s="102"/>
+      <c r="G78" s="101"/>
       <c r="H78" s="61"/>
-      <c r="I78" s="102"/>
+      <c r="I78" s="101"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" s="89" t="s">
         <v>68</v>
       </c>
       <c r="C79" s="90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D79" s="28"/>
       <c r="E79" s="28"/>
       <c r="F79" s="28"/>
-      <c r="G79" s="102"/>
+      <c r="G79" s="101"/>
       <c r="H79" s="61"/>
-      <c r="I79" s="102"/>
+      <c r="I79" s="101"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B80" s="89" t="s">
         <v>69</v>
       </c>
       <c r="C80" s="90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D80" s="28"/>
       <c r="E80" s="28"/>
       <c r="F80" s="28"/>
-      <c r="G80" s="102"/>
+      <c r="G80" s="101"/>
       <c r="H80" s="61"/>
-      <c r="I80" s="102"/>
+      <c r="I80" s="101"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B81" s="89" t="s">
         <v>64</v>
       </c>
       <c r="C81" s="90" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D81" s="28"/>
       <c r="E81" s="28"/>
       <c r="F81" s="28"/>
-      <c r="G81" s="102"/>
+      <c r="G81" s="101"/>
       <c r="H81" s="61"/>
-      <c r="I81" s="102"/>
+      <c r="I81" s="101"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B82" s="101"/>
-      <c r="C82" s="102"/>
+      <c r="B82" s="100"/>
+      <c r="C82" s="101"/>
       <c r="D82" s="28"/>
       <c r="E82" s="28"/>
       <c r="F82" s="28"/>
-      <c r="G82" s="102"/>
+      <c r="G82" s="101"/>
       <c r="H82" s="61"/>
-      <c r="I82" s="102"/>
+      <c r="I82" s="101"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B83" s="101"/>
-      <c r="C83" s="102"/>
+      <c r="B83" s="100"/>
+      <c r="C83" s="101"/>
       <c r="D83" s="28"/>
       <c r="E83" s="28"/>
       <c r="F83" s="28"/>
-      <c r="G83" s="102"/>
+      <c r="G83" s="101"/>
       <c r="H83" s="61"/>
-      <c r="I83" s="102"/>
+      <c r="I83" s="101"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B84" s="101"/>
-      <c r="C84" s="102"/>
+      <c r="B84" s="100"/>
+      <c r="C84" s="101"/>
       <c r="D84" s="28"/>
       <c r="E84" s="28"/>
       <c r="F84" s="28"/>
-      <c r="G84" s="102"/>
+      <c r="G84" s="101"/>
       <c r="H84" s="61"/>
-      <c r="I84" s="102"/>
+      <c r="I84" s="101"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B85" s="101"/>
-      <c r="C85" s="102"/>
+      <c r="B85" s="100"/>
+      <c r="C85" s="101"/>
       <c r="D85" s="28"/>
       <c r="E85" s="28"/>
       <c r="F85" s="28"/>
-      <c r="G85" s="102"/>
+      <c r="G85" s="101"/>
       <c r="H85" s="61"/>
-      <c r="I85" s="102"/>
+      <c r="I85" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9324,11 +9333,8 @@
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="G27" r:id="rId1" location="testing-user-education" display="https://github.com/OWASP/owasp-mstg/blob/1.1.0/Document/0x04i-Testing-user-interaction.md - testing-user-education" xr:uid="{3C190139-796B-A245-B60E-3DEAEE40B5CA}"/>
-  </hyperlinks>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="35" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="35" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="46" max="16383" man="1"/>
   </rowBreaks>
@@ -9351,26 +9357,26 @@
     <col min="3" max="3" width="93.1640625" style="94" customWidth="1"/>
     <col min="4" max="4" width="2.9140625" style="19" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="42.4140625" style="102" customWidth="1"/>
+    <col min="6" max="6" width="42.4140625" style="101" customWidth="1"/>
     <col min="7" max="7" width="30.58203125" style="94" customWidth="1"/>
     <col min="8" max="16384" width="10.9140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="21.6" x14ac:dyDescent="0.6">
       <c r="B1" s="93" t="s">
-        <v>283</v>
-      </c>
-      <c r="G1" s="102"/>
+        <v>282</v>
+      </c>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="102"/>
+      <c r="G2" s="101"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="49" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D3" s="51" t="s">
         <v>38</v>
@@ -9379,16 +9385,16 @@
         <v>184</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="65"/>
       <c r="C4" s="66" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D4" s="67"/>
       <c r="E4" s="67"/>
@@ -9396,11 +9402,11 @@
       <c r="G4" s="69"/>
     </row>
     <row r="5" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="107" t="s">
         <v>113</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D5" s="92" t="s">
         <v>3</v>
@@ -9418,11 +9424,11 @@
       <c r="G5" s="62"/>
     </row>
     <row r="6" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="107" t="s">
         <v>114</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D6" s="92" t="s">
         <v>3</v>
@@ -9440,11 +9446,11 @@
       <c r="G6" s="62"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="107" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="92" t="s">
         <v>3</v>
@@ -9462,11 +9468,11 @@
       <c r="G7" s="62"/>
     </row>
     <row r="8" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="107" t="s">
         <v>116</v>
       </c>
       <c r="C8" s="74" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D8" s="92" t="s">
         <v>3</v>
@@ -9480,11 +9486,11 @@
       <c r="G8" s="62"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="107" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D9" s="92" t="s">
         <v>3</v>
@@ -9498,11 +9504,11 @@
       <c r="G9" s="62"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="107" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="74" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D10" s="92" t="s">
         <v>3</v>
@@ -9516,11 +9522,11 @@
       <c r="G10" s="62"/>
     </row>
     <row r="11" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="107" t="s">
         <v>119</v>
       </c>
       <c r="C11" s="74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D11" s="92" t="s">
         <v>3</v>
@@ -9534,11 +9540,11 @@
       <c r="G11" s="62"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="107" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="74" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D12" s="92" t="s">
         <v>3</v>
@@ -9552,11 +9558,11 @@
       <c r="G12" s="62"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="107" t="s">
         <v>95</v>
       </c>
       <c r="C13" s="74" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D13" s="92" t="s">
         <v>3</v>
@@ -9572,7 +9578,7 @@
     <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="65"/>
       <c r="C14" s="66" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D14" s="67"/>
       <c r="E14" s="67"/>
@@ -9580,11 +9586,11 @@
       <c r="G14" s="69"/>
     </row>
     <row r="15" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="108" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="74" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D15" s="92" t="s">
         <v>3</v>
@@ -9604,7 +9610,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="65"/>
       <c r="C16" s="66" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D16" s="67"/>
       <c r="E16" s="67"/>
@@ -9612,11 +9618,11 @@
       <c r="G16" s="69"/>
     </row>
     <row r="17" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="107" t="s">
         <v>121</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>3</v>
@@ -9630,11 +9636,11 @@
       <c r="G17" s="62"/>
     </row>
     <row r="18" spans="2:7" ht="52.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="107" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="74" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D18" s="92" t="s">
         <v>3</v>
@@ -9656,108 +9662,108 @@
       <c r="G19" s="84"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="101"/>
-      <c r="C20" s="102"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="101"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
-      <c r="G20" s="102"/>
+      <c r="G20" s="101"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="101"/>
-      <c r="C21" s="102"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="101"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
-      <c r="G21" s="102"/>
+      <c r="G21" s="101"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="103" t="s">
-        <v>276</v>
-      </c>
-      <c r="C22" s="102"/>
+      <c r="B22" s="102" t="s">
+        <v>275</v>
+      </c>
+      <c r="C22" s="101"/>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
-      <c r="G22" s="102"/>
+      <c r="G22" s="101"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" s="88" t="s">
         <v>277</v>
-      </c>
-      <c r="C23" s="88" t="s">
-        <v>278</v>
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
-      <c r="G23" s="102"/>
+      <c r="G23" s="101"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="89" t="s">
         <v>68</v>
       </c>
       <c r="C24" s="90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
-      <c r="G24" s="102"/>
+      <c r="G24" s="101"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="89" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28"/>
-      <c r="G25" s="102"/>
+      <c r="G25" s="101"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="89" t="s">
         <v>64</v>
       </c>
       <c r="C26" s="90" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
-      <c r="G26" s="102"/>
+      <c r="G26" s="101"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="101"/>
-      <c r="C27" s="102"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="101"/>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
-      <c r="G27" s="102"/>
+      <c r="G27" s="101"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="101"/>
-      <c r="C28" s="102"/>
+      <c r="B28" s="100"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
-      <c r="G28" s="102"/>
+      <c r="G28" s="101"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="101"/>
-      <c r="C29" s="102"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="101"/>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
-      <c r="G29" s="102"/>
+      <c r="G29" s="101"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="101"/>
-      <c r="C30" s="102"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="101"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="101"/>
-      <c r="C31" s="102"/>
+      <c r="B31" s="100"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="101"/>
-      <c r="C32" s="102"/>
+      <c r="B32" s="100"/>
+      <c r="C32" s="101"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
     </row>
@@ -9818,9 +9824,9 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="84" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -9832,10 +9838,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="155"/>
+      <c r="B1" s="156"/>
       <c r="C1" s="10"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -10127,16 +10133,16 @@
         <v>124</v>
       </c>
       <c r="B20" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="C20" s="110" t="s">
         <v>288</v>
-      </c>
-      <c r="C20" s="157" t="s">
-        <v>289</v>
       </c>
       <c r="D20" s="14">
         <v>43641</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -10144,16 +10150,50 @@
         <v>124</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C21" s="157" t="s">
-        <v>100</v>
+        <v>290</v>
+      </c>
+      <c r="C21" s="110" t="s">
+        <v>288</v>
       </c>
       <c r="D21" s="14">
         <v>43642</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="C22" s="110" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="14">
+        <v>43649</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="C23" s="110" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="14">
+        <v>43672</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -10171,7 +10211,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -10186,78 +10226,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="157" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="109"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="103" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="103" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="103" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="103" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="103" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="106" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="106" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="104">
+        <v>43402</v>
+      </c>
+      <c r="E3" s="105" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="110"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="104" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="104" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="104" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="104" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="104" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="106" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="105" t="s">
         <v>177</v>
       </c>
-      <c r="B3" s="107" t="s">
-        <v>179</v>
-      </c>
-      <c r="C3" s="107" t="s">
-        <v>211</v>
-      </c>
-      <c r="D3" s="105">
-        <v>43402</v>
-      </c>
-      <c r="E3" s="106" t="s">
+      <c r="B4" s="106" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="104">
+        <v>43590</v>
+      </c>
+      <c r="E4" s="105" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="106" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="105" t="s">
         <v>177</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B5" s="106" t="s">
         <v>178</v>
       </c>
-      <c r="C4" s="107" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" s="105">
-        <v>43590</v>
-      </c>
-      <c r="E4" s="106" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="106" t="s">
+      <c r="C5" s="106" t="s">
+        <v>296</v>
+      </c>
+      <c r="D5" s="104">
+        <v>43643</v>
+      </c>
+      <c r="E5" s="105" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="105" t="s">
         <v>177</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B6" s="106" t="s">
         <v>178</v>
       </c>
-      <c r="C5" s="107" t="s">
-        <v>297</v>
-      </c>
-      <c r="D5" s="105">
-        <v>43643</v>
-      </c>
-      <c r="E5" s="106" t="s">
-        <v>298</v>
+      <c r="C6" s="106" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="104">
+        <v>43673</v>
+      </c>
+      <c r="E6" s="105" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>